<commit_message>
Atualizando planilha com dados oficiais
</commit_message>
<xml_diff>
--- a/CPlex.net/data/input.xlsx
+++ b/CPlex.net/data/input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uC249567\Dropbox\UFJF\SI\8º período SI\Pesquisa Operacional\Trabalho final\dcc163-pesquisa-operacional\CPlex.net\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uC249567\Dropbox\UFJF\SI\8º período SI\Pesquisa Operacional\Trabalho final\dcc163-pesquisa-operacional\CPlex.net\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04AEA4F8-C944-48DF-B156-438C3084A7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136A3445-C28B-4FFE-BA9B-116A04F1335A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="5070" windowWidth="21600" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Carga horária segunda</t>
   </si>
@@ -164,6 +164,54 @@
   </si>
   <si>
     <t>TOTAL DE CARGA HORÁRIA DA EQUIPE DISPONÍVEL</t>
+  </si>
+  <si>
+    <t>$0.54</t>
+  </si>
+  <si>
+    <t>$0.80</t>
+  </si>
+  <si>
+    <t>$0.67</t>
+  </si>
+  <si>
+    <t>$1.00</t>
+  </si>
+  <si>
+    <t>$0.40</t>
+  </si>
+  <si>
+    <t>$0.60</t>
+  </si>
+  <si>
+    <t>$8.04</t>
+  </si>
+  <si>
+    <t>$12.05</t>
+  </si>
+  <si>
+    <t>$0.27</t>
+  </si>
+  <si>
+    <t>$0.13</t>
+  </si>
+  <si>
+    <t>$0.20</t>
+  </si>
+  <si>
+    <t>$0.64</t>
+  </si>
+  <si>
+    <t>$0.96</t>
+  </si>
+  <si>
+    <t>$0.45</t>
+  </si>
+  <si>
+    <t>$0.43</t>
+  </si>
+  <si>
+    <t>$0.65</t>
   </si>
 </sst>
 </file>
@@ -222,12 +270,12 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +559,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,130 +577,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2">
-        <v>25</v>
-      </c>
-      <c r="D3" s="2">
-        <v>25</v>
-      </c>
-      <c r="E3" s="2">
-        <v>25</v>
-      </c>
-      <c r="F3" s="2">
+      <c r="A3" s="1">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1">
+        <v>24</v>
+      </c>
+      <c r="C3" s="1">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -660,420 +708,420 @@
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>15</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D7">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7">
         <v>2</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>6</v>
-      </c>
-      <c r="I7">
-        <v>7</v>
-      </c>
-      <c r="J7">
-        <v>8</v>
-      </c>
-      <c r="K7">
-        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>12</v>
       </c>
       <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
         <v>1</v>
       </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8">
         <v>4</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8">
-        <v>6</v>
-      </c>
-      <c r="I8">
-        <v>7</v>
-      </c>
-      <c r="J8">
-        <v>8</v>
-      </c>
-      <c r="K8">
-        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>20</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G9">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H9">
-        <v>6</v>
-      </c>
-      <c r="I9">
-        <v>7</v>
-      </c>
-      <c r="J9">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="I9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
         <v>4</v>
       </c>
-      <c r="G10">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10">
         <v>5</v>
-      </c>
-      <c r="H10">
-        <v>6</v>
-      </c>
-      <c r="I10">
-        <v>7</v>
-      </c>
-      <c r="J10">
-        <v>8</v>
-      </c>
-      <c r="K10">
-        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>12</v>
       </c>
       <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
         <v>1</v>
       </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <v>4</v>
-      </c>
       <c r="G11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H11">
         <v>6</v>
       </c>
-      <c r="I11">
-        <v>7</v>
-      </c>
-      <c r="J11">
-        <v>8</v>
+      <c r="I11" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" t="s">
+        <v>34</v>
       </c>
       <c r="K11">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>30</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F12">
+        <v>20</v>
+      </c>
+      <c r="G12">
+        <v>13</v>
+      </c>
+      <c r="H12">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12">
         <v>4</v>
-      </c>
-      <c r="G12">
-        <v>5</v>
-      </c>
-      <c r="H12">
-        <v>6</v>
-      </c>
-      <c r="I12">
-        <v>7</v>
-      </c>
-      <c r="J12">
-        <v>8</v>
-      </c>
-      <c r="K12">
-        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <v>60</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <v>25</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13">
         <v>2</v>
-      </c>
-      <c r="E13">
-        <v>3</v>
-      </c>
-      <c r="F13">
-        <v>4</v>
-      </c>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13">
-        <v>6</v>
-      </c>
-      <c r="I13">
-        <v>7</v>
-      </c>
-      <c r="J13">
-        <v>8</v>
-      </c>
-      <c r="K13">
-        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>12.5</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H14">
         <v>6</v>
       </c>
-      <c r="I14">
-        <v>7</v>
-      </c>
-      <c r="J14">
-        <v>8</v>
+      <c r="I14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" t="s">
+        <v>43</v>
       </c>
       <c r="K14">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>18</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="G15">
+        <v>22</v>
+      </c>
+      <c r="H15">
+        <v>18</v>
+      </c>
+      <c r="I15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15">
         <v>5</v>
-      </c>
-      <c r="H15">
-        <v>6</v>
-      </c>
-      <c r="I15">
-        <v>7</v>
-      </c>
-      <c r="J15">
-        <v>8</v>
-      </c>
-      <c r="K15">
-        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>12</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D16">
+        <v>24</v>
+      </c>
+      <c r="E16">
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <v>16</v>
+      </c>
+      <c r="G16">
+        <v>32</v>
+      </c>
+      <c r="H16">
+        <v>12</v>
+      </c>
+      <c r="I16" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16">
         <v>2</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="F16">
-        <v>4</v>
-      </c>
-      <c r="G16">
-        <v>5</v>
-      </c>
-      <c r="H16">
-        <v>6</v>
-      </c>
-      <c r="I16">
-        <v>7</v>
-      </c>
-      <c r="J16">
-        <v>8</v>
-      </c>
-      <c r="K16">
-        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>18.666666666666668</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G17">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H17">
         <v>6</v>
       </c>
-      <c r="I17">
-        <v>7</v>
-      </c>
-      <c r="J17">
-        <v>8</v>
+      <c r="I17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" t="s">
+        <v>46</v>
       </c>
       <c r="K17">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>12.5</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>36</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E18">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F18">
+        <v>30</v>
+      </c>
+      <c r="G18">
+        <v>42</v>
+      </c>
+      <c r="H18">
+        <v>12</v>
+      </c>
+      <c r="I18" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18">
         <v>4</v>
-      </c>
-      <c r="G18">
-        <v>5</v>
-      </c>
-      <c r="H18">
-        <v>6</v>
-      </c>
-      <c r="I18">
-        <v>7</v>
-      </c>
-      <c r="J18">
-        <v>8</v>
-      </c>
-      <c r="K18">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>